<commit_message>
some textput has been changed so that only they take integer values
</commit_message>
<xml_diff>
--- a/puffstock.xlsx
+++ b/puffstock.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I10" sqref="A1:XFD1048576"/>
@@ -520,6 +520,41 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>31413</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update order infos screen add
</commit_message>
<xml_diff>
--- a/puffstock.xlsx
+++ b/puffstock.xlsx
@@ -390,13 +390,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
@@ -723,6 +723,886 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINMADI</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINMADI</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>hasan</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINMADI</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>hasan</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>şaziye</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>23413</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>yeni</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ruhi</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>-321</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>ÖDEME ALINDI</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>26-03-2023</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
it can add products in excel
</commit_message>
<xml_diff>
--- a/puffstock.xlsx
+++ b/puffstock.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Stock" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -390,57 +391,69 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="A1:XFD1048576"/>
+      <selection activeCell="H8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="20.42578125" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>SİP_NO</t>
+          <t>TÜR</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>İSİM</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>TELEFON NO</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>ÜRÜN</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
           <t>ADET</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>ÖDEME DURUMU</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>NOT</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>SİPARİŞ TARİHİ</t>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>muz</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>elma</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>30</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
product control system completed
</commit_message>
<xml_diff>
--- a/puffstock.xlsx
+++ b/puffstock.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4695" yWindow="1935" windowWidth="21600" windowHeight="10470" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4695" yWindow="1935" windowWidth="21600" windowHeight="10470" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" state="visible" r:id="rId1"/>
@@ -393,7 +393,7 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -409,10 +409,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="A1:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -420,36 +420,77 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>PRO_N0</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>TÜR</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>ADET</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>muz</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>12</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>elma</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>30</t>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>göt</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ruvi</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>

</xml_diff>